<commit_message>
Various changes after the conf call
</commit_message>
<xml_diff>
--- a/Services commands.xlsx
+++ b/Services commands.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\Source\Repos\Teamwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="commands for engine" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Alexander:</t>
         </r>
@@ -46,7 +47,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 enum</t>
@@ -61,7 +63,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Alexander:</t>
         </r>
@@ -70,7 +73,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 from enum
@@ -86,7 +90,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Alexander:</t>
         </r>
@@ -95,7 +100,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 battery / tire/ door
@@ -111,7 +117,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Alexander:</t>
         </r>
@@ -120,7 +127,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 from enum
@@ -136,7 +144,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Alexander:</t>
         </r>
@@ -145,7 +154,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 battery / tire/ door
@@ -161,7 +171,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Alexander:</t>
         </r>
@@ -170,7 +181,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 from enum
@@ -186,7 +198,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Alexander:</t>
         </r>
@@ -195,7 +208,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 VehicleType enum = numbers of wheels</t>
@@ -207,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="78">
   <si>
     <t>addEmployee</t>
   </si>
@@ -380,9 +394,6 @@
     <t>remove Payment &amp; Credit =&gt; we have due days in Client</t>
   </si>
   <si>
-    <t>SellStock remove vehicle, might be null, client might buy stock even if he does not have a car</t>
-  </si>
-  <si>
     <t>stockId</t>
   </si>
   <si>
@@ -420,13 +431,37 @@
   </si>
   <si>
     <t>no need for IsAccepted in Sales - we set the SellService command only if it's accepted</t>
+  </si>
+  <si>
+    <t>EmployeeId</t>
+  </si>
+  <si>
+    <t>Remove IOrderService</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>Comment from discussion</t>
+  </si>
+  <si>
+    <t>Client Cost for Stock = Cost of Stock * 1.5</t>
+  </si>
+  <si>
+    <t>Команда: Списък с колина клиент</t>
+  </si>
+  <si>
+    <t>AutoserviceProfit</t>
+  </si>
+  <si>
+    <t>Service List</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,22 +474,39 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -469,15 +521,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -752,25 +834,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="51" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="51" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -786,31 +869,34 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M1" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -823,11 +909,11 @@
       <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>14</v>
       </c>
@@ -837,11 +923,14 @@
       <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="K4" t="s">
+      <c r="H4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -860,14 +949,14 @@
       <c r="F5" t="s">
         <v>42</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>21</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -886,14 +975,14 @@
       <c r="F6" t="s">
         <v>42</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>21</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -913,13 +1002,13 @@
         <v>31</v>
       </c>
       <c r="H7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" t="s">
         <v>53</v>
       </c>
-      <c r="K7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>32</v>
       </c>
@@ -935,11 +1024,14 @@
       <c r="F8" t="s">
         <v>55</v>
       </c>
-      <c r="K8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>70</v>
+      </c>
+      <c r="L8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>26</v>
       </c>
@@ -959,44 +1051,65 @@
         <v>31</v>
       </c>
       <c r="H9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" t="s">
         <v>53</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>42</v>
-      </c>
-      <c r="K10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" t="s">
-        <v>67</v>
-      </c>
-      <c r="K11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1010,13 +1123,13 @@
         <v>25</v>
       </c>
       <c r="E12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" t="s">
         <v>58</v>
       </c>
-      <c r="H12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1032,95 +1145,121 @@
       <c r="E13" t="s">
         <v>29</v>
       </c>
-      <c r="H13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="I13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="M14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>45</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>47</v>
       </c>
       <c r="E25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>49</v>
       </c>
-      <c r="E27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>51</v>
       </c>
       <c r="E29" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>